<commit_message>
refactor: importion des donnees parquet
- utilisation de la fonction left_join de dplyr pour la jointure
</commit_message>
<xml_diff>
--- a/regions/data/variables_region.xlsx
+++ b/regions/data/variables_region.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26717"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Datavizzz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FontyColoBe\Documents\GitHub\cereq-dataviz\regions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{47F3FEB3-8F1F-4EA2-9C52-3F5FCF88A8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00947EF7-C238-4F34-A195-03BB33095517}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4338D393-E209-4A28-9CF7-3BEB4D8565C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
+    <workbookView xWindow="28680" yWindow="-8355" windowWidth="29040" windowHeight="15720" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>Proportion de sortants cadres à trois ans</t>
   </si>
   <si>
-    <t>pos_prof_inter</t>
-  </si>
-  <si>
     <t>Proportion de sortants professions intermédiaires à trois ans</t>
   </si>
   <si>
@@ -165,13 +162,16 @@
   </si>
   <si>
     <t>Proportion de sortants ayant un diplôme de l'enseignement supérieur long comme plus haut diplôme</t>
+  </si>
+  <si>
+    <t>pos_prof_int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,7 +245,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -544,19 +544,19 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="1"/>
-    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="67.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="2" width="10.81640625" style="1"/>
+    <col min="3" max="3" width="23.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="67.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.54296875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -595,7 +595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -609,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -623,7 +623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -637,7 +637,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -651,7 +651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75">
+    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -693,7 +693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75">
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -704,81 +704,81 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75">
+    </row>
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75">
+    </row>
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1">
+    </row>
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>4</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -788,6 +788,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e7a409e0b47e02996c47cd99ab55c69c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ec4d4004c5339e4d0b1f4fd079361e4" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -1010,15 +1019,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1031,13 +1031,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>